<commit_message>
Incluye pacientes hasta P29 sin P27 sin P09 Habiendo corregido grupos a Diciembre 2022 Revisión de Banish List Corregido todos los rows faltantes en shor_df Listillo
Por fin armando graficos representativos!

INICIAMOS LSL_LAB grabbing

P34 LISTO
</commit_message>
<xml_diff>
--- a/AB_SimianMaze_Z2_Banished_NaviData.xlsx
+++ b/AB_SimianMaze_Z2_Banished_NaviData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J351"/>
+  <dimension ref="A1:J477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13780,6 +13780,4794 @@
         <v>1</v>
       </c>
     </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>1816</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E352" t="n">
+        <v>7</v>
+      </c>
+      <c r="F352" t="n">
+        <v>29912</v>
+      </c>
+      <c r="G352" t="n">
+        <v>1587</v>
+      </c>
+      <c r="H352" t="n">
+        <v>0</v>
+      </c>
+      <c r="I352" t="n">
+        <v>2.795084971874737</v>
+      </c>
+      <c r="J352" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>1817</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E353" t="n">
+        <v>1</v>
+      </c>
+      <c r="F353" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G353" t="n">
+        <v>468</v>
+      </c>
+      <c r="H353" t="n">
+        <v>0</v>
+      </c>
+      <c r="I353" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="J353" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>1818</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E354" t="n">
+        <v>1</v>
+      </c>
+      <c r="F354" t="n">
+        <v>30001</v>
+      </c>
+      <c r="G354" t="n">
+        <v>468</v>
+      </c>
+      <c r="H354" t="n">
+        <v>0</v>
+      </c>
+      <c r="I354" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="J354" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>1819</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E355" t="n">
+        <v>1</v>
+      </c>
+      <c r="F355" t="n">
+        <v>30002</v>
+      </c>
+      <c r="G355" t="n">
+        <v>117</v>
+      </c>
+      <c r="H355" t="n">
+        <v>0</v>
+      </c>
+      <c r="I355" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J355" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>1820</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E356" t="n">
+        <v>2</v>
+      </c>
+      <c r="F356" t="n">
+        <v>30003</v>
+      </c>
+      <c r="G356" t="n">
+        <v>117</v>
+      </c>
+      <c r="H356" t="n">
+        <v>0</v>
+      </c>
+      <c r="I356" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J356" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>1821</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E357" t="n">
+        <v>3</v>
+      </c>
+      <c r="F357" t="n">
+        <v>30004</v>
+      </c>
+      <c r="G357" t="n">
+        <v>802</v>
+      </c>
+      <c r="H357" t="n">
+        <v>0</v>
+      </c>
+      <c r="I357" t="n">
+        <v>3.365728004459064</v>
+      </c>
+      <c r="J357" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>1822</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E358" t="n">
+        <v>4</v>
+      </c>
+      <c r="F358" t="n">
+        <v>30005</v>
+      </c>
+      <c r="G358" t="n">
+        <v>117</v>
+      </c>
+      <c r="H358" t="n">
+        <v>0</v>
+      </c>
+      <c r="I358" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J358" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>1823</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E359" t="n">
+        <v>1</v>
+      </c>
+      <c r="F359" t="n">
+        <v>30006</v>
+      </c>
+      <c r="G359" t="n">
+        <v>117</v>
+      </c>
+      <c r="H359" t="n">
+        <v>0</v>
+      </c>
+      <c r="I359" t="n">
+        <v>0.1996489265624812</v>
+      </c>
+      <c r="J359" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>1824</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E360" t="n">
+        <v>2</v>
+      </c>
+      <c r="F360" t="n">
+        <v>30007</v>
+      </c>
+      <c r="G360" t="n">
+        <v>585</v>
+      </c>
+      <c r="H360" t="n">
+        <v>0</v>
+      </c>
+      <c r="I360" t="n">
+        <v>0.9982446328124059</v>
+      </c>
+      <c r="J360" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>1825</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E361" t="n">
+        <v>3</v>
+      </c>
+      <c r="F361" t="n">
+        <v>30008</v>
+      </c>
+      <c r="G361" t="n">
+        <v>468</v>
+      </c>
+      <c r="H361" t="n">
+        <v>0</v>
+      </c>
+      <c r="I361" t="n">
+        <v>0.7985957062499247</v>
+      </c>
+      <c r="J361" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>1826</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E362" t="n">
+        <v>4</v>
+      </c>
+      <c r="F362" t="n">
+        <v>30009</v>
+      </c>
+      <c r="G362" t="n">
+        <v>4476</v>
+      </c>
+      <c r="H362" t="n">
+        <v>0.08965910263666951</v>
+      </c>
+      <c r="I362" t="n">
+        <v>7.925504865962518</v>
+      </c>
+      <c r="J362" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>1827</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E363" t="n">
+        <v>5</v>
+      </c>
+      <c r="F363" t="n">
+        <v>30010</v>
+      </c>
+      <c r="G363" t="n">
+        <v>3373</v>
+      </c>
+      <c r="H363" t="n">
+        <v>0.1064241714967378</v>
+      </c>
+      <c r="I363" t="n">
+        <v>5.869289625294489</v>
+      </c>
+      <c r="J363" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>1828</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E364" t="n">
+        <v>6</v>
+      </c>
+      <c r="F364" t="n">
+        <v>30011</v>
+      </c>
+      <c r="G364" t="n">
+        <v>2037</v>
+      </c>
+      <c r="H364" t="n">
+        <v>0.09863283854969299</v>
+      </c>
+      <c r="I364" t="n">
+        <v>3.391798160963492</v>
+      </c>
+      <c r="J364" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>1847</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E365" t="n">
+        <v>1</v>
+      </c>
+      <c r="F365" t="n">
+        <v>30400</v>
+      </c>
+      <c r="G365" t="n">
+        <v>44989</v>
+      </c>
+      <c r="H365" t="n">
+        <v>1.653073880042522</v>
+      </c>
+      <c r="I365" t="n">
+        <v>110.7579747577465</v>
+      </c>
+      <c r="J365" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>1848</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E366" t="n">
+        <v>1</v>
+      </c>
+      <c r="F366" t="n">
+        <v>30500</v>
+      </c>
+      <c r="G366" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H366" t="n">
+        <v>0</v>
+      </c>
+      <c r="I366" t="n">
+        <v>2.410714285714285</v>
+      </c>
+      <c r="J366" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>1849</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E367" t="n">
+        <v>1</v>
+      </c>
+      <c r="F367" t="n">
+        <v>30501</v>
+      </c>
+      <c r="G367" t="n">
+        <v>42100</v>
+      </c>
+      <c r="H367" t="n">
+        <v>0.001029391931029434</v>
+      </c>
+      <c r="I367" t="n">
+        <v>101.2706762072299</v>
+      </c>
+      <c r="J367" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E368" t="n">
+        <v>3</v>
+      </c>
+      <c r="F368" t="n">
+        <v>30608</v>
+      </c>
+      <c r="G368" t="n">
+        <v>41111</v>
+      </c>
+      <c r="H368" t="n">
+        <v>1.657205714486827</v>
+      </c>
+      <c r="I368" t="n">
+        <v>82.38944738609995</v>
+      </c>
+      <c r="J368" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>1859</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E369" t="n">
+        <v>1</v>
+      </c>
+      <c r="F369" t="n">
+        <v>30700</v>
+      </c>
+      <c r="G369" t="n">
+        <v>556</v>
+      </c>
+      <c r="H369" t="n">
+        <v>0</v>
+      </c>
+      <c r="I369" t="n">
+        <v>1.339285714285714</v>
+      </c>
+      <c r="J369" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>1860</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E370" t="n">
+        <v>1</v>
+      </c>
+      <c r="F370" t="n">
+        <v>30800</v>
+      </c>
+      <c r="G370" t="n">
+        <v>444</v>
+      </c>
+      <c r="H370" t="n">
+        <v>0</v>
+      </c>
+      <c r="I370" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="J370" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>1861</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E371" t="n">
+        <v>1</v>
+      </c>
+      <c r="F371" t="n">
+        <v>30801</v>
+      </c>
+      <c r="G371" t="n">
+        <v>222</v>
+      </c>
+      <c r="H371" t="n">
+        <v>0</v>
+      </c>
+      <c r="I371" t="n">
+        <v>0.5357142857142856</v>
+      </c>
+      <c r="J371" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>1862</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E372" t="n">
+        <v>1</v>
+      </c>
+      <c r="F372" t="n">
+        <v>30802</v>
+      </c>
+      <c r="G372" t="n">
+        <v>1111</v>
+      </c>
+      <c r="H372" t="n">
+        <v>0.01498046225151983</v>
+      </c>
+      <c r="I372" t="n">
+        <v>4.80894915711524</v>
+      </c>
+      <c r="J372" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>1863</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E373" t="n">
+        <v>1</v>
+      </c>
+      <c r="F373" t="n">
+        <v>30900</v>
+      </c>
+      <c r="G373" t="n">
+        <v>111</v>
+      </c>
+      <c r="H373" t="n">
+        <v>0</v>
+      </c>
+      <c r="I373" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J373" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>1864</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E374" t="n">
+        <v>1</v>
+      </c>
+      <c r="F374" t="n">
+        <v>30901</v>
+      </c>
+      <c r="G374" t="n">
+        <v>111</v>
+      </c>
+      <c r="H374" t="n">
+        <v>0</v>
+      </c>
+      <c r="I374" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J374" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>1865</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E375" t="n">
+        <v>1</v>
+      </c>
+      <c r="F375" t="n">
+        <v>30902</v>
+      </c>
+      <c r="G375" t="n">
+        <v>111</v>
+      </c>
+      <c r="H375" t="n">
+        <v>0</v>
+      </c>
+      <c r="I375" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J375" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>1866</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E376" t="n">
+        <v>2</v>
+      </c>
+      <c r="F376" t="n">
+        <v>30903</v>
+      </c>
+      <c r="G376" t="n">
+        <v>333</v>
+      </c>
+      <c r="H376" t="n">
+        <v>0</v>
+      </c>
+      <c r="I376" t="n">
+        <v>1.442454859053884</v>
+      </c>
+      <c r="J376" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>1867</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E377" t="n">
+        <v>3</v>
+      </c>
+      <c r="F377" t="n">
+        <v>30904</v>
+      </c>
+      <c r="G377" t="n">
+        <v>111</v>
+      </c>
+      <c r="H377" t="n">
+        <v>0</v>
+      </c>
+      <c r="I377" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J377" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>1868</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E378" t="n">
+        <v>4</v>
+      </c>
+      <c r="F378" t="n">
+        <v>30905</v>
+      </c>
+      <c r="G378" t="n">
+        <v>1778</v>
+      </c>
+      <c r="H378" t="n">
+        <v>0</v>
+      </c>
+      <c r="I378" t="n">
+        <v>7.693092581620717</v>
+      </c>
+      <c r="J378" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>1869</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E379" t="n">
+        <v>1</v>
+      </c>
+      <c r="F379" t="n">
+        <v>30906</v>
+      </c>
+      <c r="G379" t="n">
+        <v>111</v>
+      </c>
+      <c r="H379" t="n">
+        <v>0</v>
+      </c>
+      <c r="I379" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J379" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>1870</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E380" t="n">
+        <v>1</v>
+      </c>
+      <c r="F380" t="n">
+        <v>31000</v>
+      </c>
+      <c r="G380" t="n">
+        <v>1111</v>
+      </c>
+      <c r="H380" t="n">
+        <v>0</v>
+      </c>
+      <c r="I380" t="n">
+        <v>2.678571428571428</v>
+      </c>
+      <c r="J380" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>1871</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E381" t="n">
+        <v>1</v>
+      </c>
+      <c r="F381" t="n">
+        <v>31001</v>
+      </c>
+      <c r="G381" t="n">
+        <v>111</v>
+      </c>
+      <c r="H381" t="n">
+        <v>0</v>
+      </c>
+      <c r="I381" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J381" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>1872</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E382" t="n">
+        <v>1</v>
+      </c>
+      <c r="F382" t="n">
+        <v>31002</v>
+      </c>
+      <c r="G382" t="n">
+        <v>111</v>
+      </c>
+      <c r="H382" t="n">
+        <v>0</v>
+      </c>
+      <c r="I382" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J382" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="n">
+        <v>1873</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E383" t="n">
+        <v>2</v>
+      </c>
+      <c r="F383" t="n">
+        <v>31003</v>
+      </c>
+      <c r="G383" t="n">
+        <v>222</v>
+      </c>
+      <c r="H383" t="n">
+        <v>0</v>
+      </c>
+      <c r="I383" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J383" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="n">
+        <v>1874</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E384" t="n">
+        <v>3</v>
+      </c>
+      <c r="F384" t="n">
+        <v>31004</v>
+      </c>
+      <c r="G384" t="n">
+        <v>111</v>
+      </c>
+      <c r="H384" t="n">
+        <v>0</v>
+      </c>
+      <c r="I384" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J384" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="n">
+        <v>1875</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E385" t="n">
+        <v>4</v>
+      </c>
+      <c r="F385" t="n">
+        <v>31005</v>
+      </c>
+      <c r="G385" t="n">
+        <v>111</v>
+      </c>
+      <c r="H385" t="n">
+        <v>0</v>
+      </c>
+      <c r="I385" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J385" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="n">
+        <v>1876</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E386" t="n">
+        <v>1</v>
+      </c>
+      <c r="F386" t="n">
+        <v>31006</v>
+      </c>
+      <c r="G386" t="n">
+        <v>444</v>
+      </c>
+      <c r="H386" t="n">
+        <v>0</v>
+      </c>
+      <c r="I386" t="n">
+        <v>1.923273145405179</v>
+      </c>
+      <c r="J386" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="n">
+        <v>1877</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E387" t="n">
+        <v>2</v>
+      </c>
+      <c r="F387" t="n">
+        <v>31007</v>
+      </c>
+      <c r="G387" t="n">
+        <v>4333</v>
+      </c>
+      <c r="H387" t="n">
+        <v>0.02066917647452639</v>
+      </c>
+      <c r="I387" t="n">
+        <v>18.68515452072871</v>
+      </c>
+      <c r="J387" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="n">
+        <v>1884</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E388" t="n">
+        <v>2</v>
+      </c>
+      <c r="F388" t="n">
+        <v>31101</v>
+      </c>
+      <c r="G388" t="n">
+        <v>20778</v>
+      </c>
+      <c r="H388" t="n">
+        <v>1.135493801827655</v>
+      </c>
+      <c r="I388" t="n">
+        <v>82.24692777419692</v>
+      </c>
+      <c r="J388" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="n">
+        <v>1886</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E389" t="n">
+        <v>1</v>
+      </c>
+      <c r="F389" t="n">
+        <v>31200</v>
+      </c>
+      <c r="G389" t="n">
+        <v>889</v>
+      </c>
+      <c r="H389" t="n">
+        <v>0</v>
+      </c>
+      <c r="I389" t="n">
+        <v>3.846546290810358</v>
+      </c>
+      <c r="J389" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="n">
+        <v>1887</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E390" t="n">
+        <v>2</v>
+      </c>
+      <c r="F390" t="n">
+        <v>31201</v>
+      </c>
+      <c r="G390" t="n">
+        <v>111</v>
+      </c>
+      <c r="H390" t="n">
+        <v>0</v>
+      </c>
+      <c r="I390" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J390" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="n">
+        <v>1888</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E391" t="n">
+        <v>3</v>
+      </c>
+      <c r="F391" t="n">
+        <v>31202</v>
+      </c>
+      <c r="G391" t="n">
+        <v>111</v>
+      </c>
+      <c r="H391" t="n">
+        <v>0</v>
+      </c>
+      <c r="I391" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J391" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="n">
+        <v>1889</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E392" t="n">
+        <v>4</v>
+      </c>
+      <c r="F392" t="n">
+        <v>31203</v>
+      </c>
+      <c r="G392" t="n">
+        <v>222</v>
+      </c>
+      <c r="H392" t="n">
+        <v>0</v>
+      </c>
+      <c r="I392" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J392" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="n">
+        <v>1890</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E393" t="n">
+        <v>5</v>
+      </c>
+      <c r="F393" t="n">
+        <v>31204</v>
+      </c>
+      <c r="G393" t="n">
+        <v>111</v>
+      </c>
+      <c r="H393" t="n">
+        <v>0</v>
+      </c>
+      <c r="I393" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J393" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="n">
+        <v>1891</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E394" t="n">
+        <v>6</v>
+      </c>
+      <c r="F394" t="n">
+        <v>31205</v>
+      </c>
+      <c r="G394" t="n">
+        <v>111</v>
+      </c>
+      <c r="H394" t="n">
+        <v>0</v>
+      </c>
+      <c r="I394" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J394" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="n">
+        <v>1892</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E395" t="n">
+        <v>7</v>
+      </c>
+      <c r="F395" t="n">
+        <v>31206</v>
+      </c>
+      <c r="G395" t="n">
+        <v>111</v>
+      </c>
+      <c r="H395" t="n">
+        <v>0</v>
+      </c>
+      <c r="I395" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J395" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="n">
+        <v>1893</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E396" t="n">
+        <v>1</v>
+      </c>
+      <c r="F396" t="n">
+        <v>31300</v>
+      </c>
+      <c r="G396" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H396" t="n">
+        <v>0</v>
+      </c>
+      <c r="I396" t="n">
+        <v>25.96418746296989</v>
+      </c>
+      <c r="J396" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>1895</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E397" t="n">
+        <v>3</v>
+      </c>
+      <c r="F397" t="n">
+        <v>31302</v>
+      </c>
+      <c r="G397" t="n">
+        <v>7000</v>
+      </c>
+      <c r="H397" t="n">
+        <v>0.4445207699666006</v>
+      </c>
+      <c r="I397" t="n">
+        <v>25.23539420146178</v>
+      </c>
+      <c r="J397" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>1940</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E398" t="n">
+        <v>1</v>
+      </c>
+      <c r="F398" t="n">
+        <v>32200</v>
+      </c>
+      <c r="G398" t="n">
+        <v>8667</v>
+      </c>
+      <c r="H398" t="n">
+        <v>0.0292502251940997</v>
+      </c>
+      <c r="I398" t="n">
+        <v>37.09827251352338</v>
+      </c>
+      <c r="J398" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>1966</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E399" t="n">
+        <v>7</v>
+      </c>
+      <c r="F399" t="n">
+        <v>32506</v>
+      </c>
+      <c r="G399" t="n">
+        <v>5260</v>
+      </c>
+      <c r="H399" t="n">
+        <v>0.1650343868609229</v>
+      </c>
+      <c r="I399" t="n">
+        <v>12.71789894801666</v>
+      </c>
+      <c r="J399" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E400" t="n">
+        <v>1</v>
+      </c>
+      <c r="F400" t="n">
+        <v>32600</v>
+      </c>
+      <c r="G400" t="n">
+        <v>919</v>
+      </c>
+      <c r="H400" t="n">
+        <v>0</v>
+      </c>
+      <c r="I400" t="n">
+        <v>1.594604356098136</v>
+      </c>
+      <c r="J400" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>1968</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E401" t="n">
+        <v>2</v>
+      </c>
+      <c r="F401" t="n">
+        <v>32601</v>
+      </c>
+      <c r="G401" t="n">
+        <v>117</v>
+      </c>
+      <c r="H401" t="n">
+        <v>0</v>
+      </c>
+      <c r="I401" t="n">
+        <v>0.5240788621767818</v>
+      </c>
+      <c r="J401" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E402" t="n">
+        <v>3</v>
+      </c>
+      <c r="F402" t="n">
+        <v>32602</v>
+      </c>
+      <c r="G402" t="n">
+        <v>117</v>
+      </c>
+      <c r="H402" t="n">
+        <v>0</v>
+      </c>
+      <c r="I402" t="n">
+        <v>0.2525557924937865</v>
+      </c>
+      <c r="J402" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E403" t="n">
+        <v>4</v>
+      </c>
+      <c r="F403" t="n">
+        <v>32603</v>
+      </c>
+      <c r="G403" t="n">
+        <v>117</v>
+      </c>
+      <c r="H403" t="n">
+        <v>0</v>
+      </c>
+      <c r="I403" t="n">
+        <v>0.1652509094980799</v>
+      </c>
+      <c r="J403" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>1971</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E404" t="n">
+        <v>5</v>
+      </c>
+      <c r="F404" t="n">
+        <v>32604</v>
+      </c>
+      <c r="G404" t="n">
+        <v>117</v>
+      </c>
+      <c r="H404" t="n">
+        <v>0</v>
+      </c>
+      <c r="I404" t="n">
+        <v>0.2603194185436162</v>
+      </c>
+      <c r="J404" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>1972</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E405" t="n">
+        <v>6</v>
+      </c>
+      <c r="F405" t="n">
+        <v>32605</v>
+      </c>
+      <c r="G405" t="n">
+        <v>234</v>
+      </c>
+      <c r="H405" t="n">
+        <v>0</v>
+      </c>
+      <c r="I405" t="n">
+        <v>0.925619536164822</v>
+      </c>
+      <c r="J405" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E406" t="n">
+        <v>1</v>
+      </c>
+      <c r="F406" t="n">
+        <v>32900</v>
+      </c>
+      <c r="G406" t="n">
+        <v>333</v>
+      </c>
+      <c r="H406" t="n">
+        <v>0</v>
+      </c>
+      <c r="I406" t="n">
+        <v>0.8035714285714284</v>
+      </c>
+      <c r="J406" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E407" t="n">
+        <v>1</v>
+      </c>
+      <c r="F407" t="n">
+        <v>33800</v>
+      </c>
+      <c r="G407" t="n">
+        <v>444</v>
+      </c>
+      <c r="H407" t="n">
+        <v>0</v>
+      </c>
+      <c r="I407" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="J407" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E408" t="n">
+        <v>1</v>
+      </c>
+      <c r="F408" t="n">
+        <v>33900</v>
+      </c>
+      <c r="G408" t="n">
+        <v>44989</v>
+      </c>
+      <c r="H408" t="n">
+        <v>2.771619669508029</v>
+      </c>
+      <c r="I408" t="n">
+        <v>85.40998343054916</v>
+      </c>
+      <c r="J408" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E409" t="n">
+        <v>1</v>
+      </c>
+      <c r="F409" t="n">
+        <v>34000</v>
+      </c>
+      <c r="G409" t="n">
+        <v>4778</v>
+      </c>
+      <c r="H409" t="n">
+        <v>0.006634039105499068</v>
+      </c>
+      <c r="I409" t="n">
+        <v>11.51930745013514</v>
+      </c>
+      <c r="J409" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E410" t="n">
+        <v>1</v>
+      </c>
+      <c r="F410" t="n">
+        <v>34100</v>
+      </c>
+      <c r="G410" t="n">
+        <v>222</v>
+      </c>
+      <c r="H410" t="n">
+        <v>0</v>
+      </c>
+      <c r="I410" t="n">
+        <v>0.5357142857142856</v>
+      </c>
+      <c r="J410" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E411" t="n">
+        <v>1</v>
+      </c>
+      <c r="F411" t="n">
+        <v>34101</v>
+      </c>
+      <c r="G411" t="n">
+        <v>444</v>
+      </c>
+      <c r="H411" t="n">
+        <v>0</v>
+      </c>
+      <c r="I411" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="J411" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E412" t="n">
+        <v>1</v>
+      </c>
+      <c r="F412" t="n">
+        <v>34200</v>
+      </c>
+      <c r="G412" t="n">
+        <v>111</v>
+      </c>
+      <c r="H412" t="n">
+        <v>0</v>
+      </c>
+      <c r="I412" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J412" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E413" t="n">
+        <v>1</v>
+      </c>
+      <c r="F413" t="n">
+        <v>34300</v>
+      </c>
+      <c r="G413" t="n">
+        <v>111</v>
+      </c>
+      <c r="H413" t="n">
+        <v>0</v>
+      </c>
+      <c r="I413" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J413" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E414" t="n">
+        <v>1</v>
+      </c>
+      <c r="F414" t="n">
+        <v>34301</v>
+      </c>
+      <c r="G414" t="n">
+        <v>111</v>
+      </c>
+      <c r="H414" t="n">
+        <v>0</v>
+      </c>
+      <c r="I414" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J414" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E415" t="n">
+        <v>1</v>
+      </c>
+      <c r="F415" t="n">
+        <v>34302</v>
+      </c>
+      <c r="G415" t="n">
+        <v>111</v>
+      </c>
+      <c r="H415" t="n">
+        <v>0</v>
+      </c>
+      <c r="I415" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J415" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E416" t="n">
+        <v>2</v>
+      </c>
+      <c r="F416" t="n">
+        <v>34303</v>
+      </c>
+      <c r="G416" t="n">
+        <v>111</v>
+      </c>
+      <c r="H416" t="n">
+        <v>0</v>
+      </c>
+      <c r="I416" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J416" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E417" t="n">
+        <v>3</v>
+      </c>
+      <c r="F417" t="n">
+        <v>34304</v>
+      </c>
+      <c r="G417" t="n">
+        <v>111</v>
+      </c>
+      <c r="H417" t="n">
+        <v>0</v>
+      </c>
+      <c r="I417" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J417" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E418" t="n">
+        <v>4</v>
+      </c>
+      <c r="F418" t="n">
+        <v>34305</v>
+      </c>
+      <c r="G418" t="n">
+        <v>111</v>
+      </c>
+      <c r="H418" t="n">
+        <v>0</v>
+      </c>
+      <c r="I418" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J418" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E419" t="n">
+        <v>1</v>
+      </c>
+      <c r="F419" t="n">
+        <v>34306</v>
+      </c>
+      <c r="G419" t="n">
+        <v>111</v>
+      </c>
+      <c r="H419" t="n">
+        <v>0</v>
+      </c>
+      <c r="I419" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J419" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E420" t="n">
+        <v>2</v>
+      </c>
+      <c r="F420" t="n">
+        <v>34307</v>
+      </c>
+      <c r="G420" t="n">
+        <v>111</v>
+      </c>
+      <c r="H420" t="n">
+        <v>0</v>
+      </c>
+      <c r="I420" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J420" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E421" t="n">
+        <v>3</v>
+      </c>
+      <c r="F421" t="n">
+        <v>34308</v>
+      </c>
+      <c r="G421" t="n">
+        <v>111</v>
+      </c>
+      <c r="H421" t="n">
+        <v>0</v>
+      </c>
+      <c r="I421" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J421" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E422" t="n">
+        <v>4</v>
+      </c>
+      <c r="F422" t="n">
+        <v>34309</v>
+      </c>
+      <c r="G422" t="n">
+        <v>111</v>
+      </c>
+      <c r="H422" t="n">
+        <v>0</v>
+      </c>
+      <c r="I422" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J422" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E423" t="n">
+        <v>5</v>
+      </c>
+      <c r="F423" t="n">
+        <v>34310</v>
+      </c>
+      <c r="G423" t="n">
+        <v>222</v>
+      </c>
+      <c r="H423" t="n">
+        <v>0</v>
+      </c>
+      <c r="I423" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J423" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1" t="n">
+        <v>2063</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>P32</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E424" t="n">
+        <v>1</v>
+      </c>
+      <c r="F424" t="n">
+        <v>34400</v>
+      </c>
+      <c r="G424" t="n">
+        <v>11000</v>
+      </c>
+      <c r="H424" t="n">
+        <v>0.6347744703986652</v>
+      </c>
+      <c r="I424" t="n">
+        <v>45.26682288443948</v>
+      </c>
+      <c r="J424" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1" t="n">
+        <v>2094</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E425" t="n">
+        <v>1</v>
+      </c>
+      <c r="F425" t="n">
+        <v>34900</v>
+      </c>
+      <c r="G425" t="n">
+        <v>47195</v>
+      </c>
+      <c r="H425" t="n">
+        <v>0</v>
+      </c>
+      <c r="I425" t="n">
+        <v>113.303571428571</v>
+      </c>
+      <c r="J425" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1" t="n">
+        <v>2102</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E426" t="n">
+        <v>1</v>
+      </c>
+      <c r="F426" t="n">
+        <v>35100</v>
+      </c>
+      <c r="G426" t="n">
+        <v>10154</v>
+      </c>
+      <c r="H426" t="n">
+        <v>0.5642264893093508</v>
+      </c>
+      <c r="I426" t="n">
+        <v>15.4273838239819</v>
+      </c>
+      <c r="J426" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1" t="n">
+        <v>2109</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>No Inmersivo</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E427" t="n">
+        <v>1</v>
+      </c>
+      <c r="F427" t="n">
+        <v>35300</v>
+      </c>
+      <c r="G427" t="n">
+        <v>16499</v>
+      </c>
+      <c r="H427" t="n">
+        <v>0.6153700126508473</v>
+      </c>
+      <c r="I427" t="n">
+        <v>74.53631007915911</v>
+      </c>
+      <c r="J427" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1" t="n">
+        <v>2130</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E428" t="n">
+        <v>1</v>
+      </c>
+      <c r="F428" t="n">
+        <v>35700</v>
+      </c>
+      <c r="G428" t="n">
+        <v>3111</v>
+      </c>
+      <c r="H428" t="n">
+        <v>0</v>
+      </c>
+      <c r="I428" t="n">
+        <v>13.46291201783625</v>
+      </c>
+      <c r="J428" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E429" t="n">
+        <v>2</v>
+      </c>
+      <c r="F429" t="n">
+        <v>35701</v>
+      </c>
+      <c r="G429" t="n">
+        <v>889</v>
+      </c>
+      <c r="H429" t="n">
+        <v>0</v>
+      </c>
+      <c r="I429" t="n">
+        <v>3.846546290810358</v>
+      </c>
+      <c r="J429" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1" t="n">
+        <v>2132</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E430" t="n">
+        <v>3</v>
+      </c>
+      <c r="F430" t="n">
+        <v>35702</v>
+      </c>
+      <c r="G430" t="n">
+        <v>444</v>
+      </c>
+      <c r="H430" t="n">
+        <v>0</v>
+      </c>
+      <c r="I430" t="n">
+        <v>1.923273145405179</v>
+      </c>
+      <c r="J430" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1" t="n">
+        <v>2133</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E431" t="n">
+        <v>4</v>
+      </c>
+      <c r="F431" t="n">
+        <v>35703</v>
+      </c>
+      <c r="G431" t="n">
+        <v>15333</v>
+      </c>
+      <c r="H431" t="n">
+        <v>0.6416619716935394</v>
+      </c>
+      <c r="I431" t="n">
+        <v>63.74452387536056</v>
+      </c>
+      <c r="J431" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1" t="n">
+        <v>2176</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E432" t="n">
+        <v>1</v>
+      </c>
+      <c r="F432" t="n">
+        <v>36500</v>
+      </c>
+      <c r="G432" t="n">
+        <v>10111</v>
+      </c>
+      <c r="H432" t="n">
+        <v>0.2367820505125625</v>
+      </c>
+      <c r="I432" t="n">
+        <v>34.91587624315078</v>
+      </c>
+      <c r="J432" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1" t="n">
+        <v>2177</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E433" t="n">
+        <v>1</v>
+      </c>
+      <c r="F433" t="n">
+        <v>36600</v>
+      </c>
+      <c r="G433" t="n">
+        <v>44989</v>
+      </c>
+      <c r="H433" t="n">
+        <v>1.682902065024234</v>
+      </c>
+      <c r="I433" t="n">
+        <v>70.60684116654686</v>
+      </c>
+      <c r="J433" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1" t="n">
+        <v>2179</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E434" t="n">
+        <v>1</v>
+      </c>
+      <c r="F434" t="n">
+        <v>36700</v>
+      </c>
+      <c r="G434" t="n">
+        <v>1556</v>
+      </c>
+      <c r="H434" t="n">
+        <v>0</v>
+      </c>
+      <c r="I434" t="n">
+        <v>3.749999999999999</v>
+      </c>
+      <c r="J434" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1" t="n">
+        <v>2180</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E435" t="n">
+        <v>1</v>
+      </c>
+      <c r="F435" t="n">
+        <v>36701</v>
+      </c>
+      <c r="G435" t="n">
+        <v>222</v>
+      </c>
+      <c r="H435" t="n">
+        <v>0</v>
+      </c>
+      <c r="I435" t="n">
+        <v>0.5357142857142856</v>
+      </c>
+      <c r="J435" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1" t="n">
+        <v>2196</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E436" t="n">
+        <v>1</v>
+      </c>
+      <c r="F436" t="n">
+        <v>36900</v>
+      </c>
+      <c r="G436" t="n">
+        <v>4778</v>
+      </c>
+      <c r="H436" t="n">
+        <v>0</v>
+      </c>
+      <c r="I436" t="n">
+        <v>20.67518631310566</v>
+      </c>
+      <c r="J436" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1" t="n">
+        <v>2197</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E437" t="n">
+        <v>2</v>
+      </c>
+      <c r="F437" t="n">
+        <v>36901</v>
+      </c>
+      <c r="G437" t="n">
+        <v>222</v>
+      </c>
+      <c r="H437" t="n">
+        <v>0</v>
+      </c>
+      <c r="I437" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J437" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1" t="n">
+        <v>2198</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E438" t="n">
+        <v>3</v>
+      </c>
+      <c r="F438" t="n">
+        <v>36902</v>
+      </c>
+      <c r="G438" t="n">
+        <v>222</v>
+      </c>
+      <c r="H438" t="n">
+        <v>0</v>
+      </c>
+      <c r="I438" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J438" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="n">
+        <v>2199</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>HiddenTarget_2</t>
+        </is>
+      </c>
+      <c r="E439" t="n">
+        <v>4</v>
+      </c>
+      <c r="F439" t="n">
+        <v>36903</v>
+      </c>
+      <c r="G439" t="n">
+        <v>778</v>
+      </c>
+      <c r="H439" t="n">
+        <v>0</v>
+      </c>
+      <c r="I439" t="n">
+        <v>3.365728004459064</v>
+      </c>
+      <c r="J439" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1" t="n">
+        <v>2209</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E440" t="n">
+        <v>7</v>
+      </c>
+      <c r="F440" t="n">
+        <v>37006</v>
+      </c>
+      <c r="G440" t="n">
+        <v>2333</v>
+      </c>
+      <c r="H440" t="n">
+        <v>0.08299182711803506</v>
+      </c>
+      <c r="I440" t="n">
+        <v>3.660472718837613</v>
+      </c>
+      <c r="J440" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1" t="n">
+        <v>2210</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E441" t="n">
+        <v>1</v>
+      </c>
+      <c r="F441" t="n">
+        <v>37100</v>
+      </c>
+      <c r="G441" t="n">
+        <v>1222</v>
+      </c>
+      <c r="H441" t="n">
+        <v>0</v>
+      </c>
+      <c r="I441" t="n">
+        <v>4.481979663800791</v>
+      </c>
+      <c r="J441" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1" t="n">
+        <v>2211</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E442" t="n">
+        <v>2</v>
+      </c>
+      <c r="F442" t="n">
+        <v>37101</v>
+      </c>
+      <c r="G442" t="n">
+        <v>222</v>
+      </c>
+      <c r="H442" t="n">
+        <v>0</v>
+      </c>
+      <c r="I442" t="n">
+        <v>1.045819412229289</v>
+      </c>
+      <c r="J442" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="1" t="n">
+        <v>2212</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E443" t="n">
+        <v>3</v>
+      </c>
+      <c r="F443" t="n">
+        <v>37102</v>
+      </c>
+      <c r="G443" t="n">
+        <v>222</v>
+      </c>
+      <c r="H443" t="n">
+        <v>0</v>
+      </c>
+      <c r="I443" t="n">
+        <v>0.440599161066631</v>
+      </c>
+      <c r="J443" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="1" t="n">
+        <v>2213</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E444" t="n">
+        <v>4</v>
+      </c>
+      <c r="F444" t="n">
+        <v>37103</v>
+      </c>
+      <c r="G444" t="n">
+        <v>111</v>
+      </c>
+      <c r="H444" t="n">
+        <v>0</v>
+      </c>
+      <c r="I444" t="n">
+        <v>0.3772865523213806</v>
+      </c>
+      <c r="J444" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="1" t="n">
+        <v>2214</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E445" t="n">
+        <v>5</v>
+      </c>
+      <c r="F445" t="n">
+        <v>37104</v>
+      </c>
+      <c r="G445" t="n">
+        <v>222</v>
+      </c>
+      <c r="H445" t="n">
+        <v>0</v>
+      </c>
+      <c r="I445" t="n">
+        <v>0.8847769931764242</v>
+      </c>
+      <c r="J445" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="1" t="n">
+        <v>2215</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>P34</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>HiddenTarget_3</t>
+        </is>
+      </c>
+      <c r="E446" t="n">
+        <v>6</v>
+      </c>
+      <c r="F446" t="n">
+        <v>37105</v>
+      </c>
+      <c r="G446" t="n">
+        <v>444</v>
+      </c>
+      <c r="H446" t="n">
+        <v>0</v>
+      </c>
+      <c r="I446" t="n">
+        <v>1.854799145228818</v>
+      </c>
+      <c r="J446" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1" t="n">
+        <v>2258</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E447" t="n">
+        <v>1</v>
+      </c>
+      <c r="F447" t="n">
+        <v>37800</v>
+      </c>
+      <c r="G447" t="n">
+        <v>667</v>
+      </c>
+      <c r="H447" t="n">
+        <v>0</v>
+      </c>
+      <c r="I447" t="n">
+        <v>1.607142857142857</v>
+      </c>
+      <c r="J447" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1" t="n">
+        <v>2259</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E448" t="n">
+        <v>1</v>
+      </c>
+      <c r="F448" t="n">
+        <v>37801</v>
+      </c>
+      <c r="G448" t="n">
+        <v>1444</v>
+      </c>
+      <c r="H448" t="n">
+        <v>0</v>
+      </c>
+      <c r="I448" t="n">
+        <v>3.482142857142856</v>
+      </c>
+      <c r="J448" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1" t="n">
+        <v>2260</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E449" t="n">
+        <v>1</v>
+      </c>
+      <c r="F449" t="n">
+        <v>37802</v>
+      </c>
+      <c r="G449" t="n">
+        <v>444</v>
+      </c>
+      <c r="H449" t="n">
+        <v>0</v>
+      </c>
+      <c r="I449" t="n">
+        <v>1.923273145405179</v>
+      </c>
+      <c r="J449" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1" t="n">
+        <v>2261</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E450" t="n">
+        <v>2</v>
+      </c>
+      <c r="F450" t="n">
+        <v>37803</v>
+      </c>
+      <c r="G450" t="n">
+        <v>333</v>
+      </c>
+      <c r="H450" t="n">
+        <v>0</v>
+      </c>
+      <c r="I450" t="n">
+        <v>1.442454859053884</v>
+      </c>
+      <c r="J450" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1" t="n">
+        <v>2262</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E451" t="n">
+        <v>3</v>
+      </c>
+      <c r="F451" t="n">
+        <v>37804</v>
+      </c>
+      <c r="G451" t="n">
+        <v>444</v>
+      </c>
+      <c r="H451" t="n">
+        <v>0</v>
+      </c>
+      <c r="I451" t="n">
+        <v>1.923273145405179</v>
+      </c>
+      <c r="J451" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="n">
+        <v>2263</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E452" t="n">
+        <v>4</v>
+      </c>
+      <c r="F452" t="n">
+        <v>37805</v>
+      </c>
+      <c r="G452" t="n">
+        <v>111</v>
+      </c>
+      <c r="H452" t="n">
+        <v>0</v>
+      </c>
+      <c r="I452" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J452" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1" t="n">
+        <v>2264</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E453" t="n">
+        <v>1</v>
+      </c>
+      <c r="F453" t="n">
+        <v>37806</v>
+      </c>
+      <c r="G453" t="n">
+        <v>222</v>
+      </c>
+      <c r="H453" t="n">
+        <v>0</v>
+      </c>
+      <c r="I453" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J453" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1" t="n">
+        <v>2265</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E454" t="n">
+        <v>2</v>
+      </c>
+      <c r="F454" t="n">
+        <v>37807</v>
+      </c>
+      <c r="G454" t="n">
+        <v>222</v>
+      </c>
+      <c r="H454" t="n">
+        <v>0</v>
+      </c>
+      <c r="I454" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J454" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1" t="n">
+        <v>2266</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E455" t="n">
+        <v>3</v>
+      </c>
+      <c r="F455" t="n">
+        <v>37808</v>
+      </c>
+      <c r="G455" t="n">
+        <v>111</v>
+      </c>
+      <c r="H455" t="n">
+        <v>0</v>
+      </c>
+      <c r="I455" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J455" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="n">
+        <v>2269</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E456" t="n">
+        <v>1</v>
+      </c>
+      <c r="F456" t="n">
+        <v>37900</v>
+      </c>
+      <c r="G456" t="n">
+        <v>889</v>
+      </c>
+      <c r="H456" t="n">
+        <v>0</v>
+      </c>
+      <c r="I456" t="n">
+        <v>2.142857142857142</v>
+      </c>
+      <c r="J456" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="n">
+        <v>2270</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E457" t="n">
+        <v>1</v>
+      </c>
+      <c r="F457" t="n">
+        <v>37901</v>
+      </c>
+      <c r="G457" t="n">
+        <v>333</v>
+      </c>
+      <c r="H457" t="n">
+        <v>0</v>
+      </c>
+      <c r="I457" t="n">
+        <v>0.8035714285714284</v>
+      </c>
+      <c r="J457" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="n">
+        <v>2271</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E458" t="n">
+        <v>1</v>
+      </c>
+      <c r="F458" t="n">
+        <v>37902</v>
+      </c>
+      <c r="G458" t="n">
+        <v>111</v>
+      </c>
+      <c r="H458" t="n">
+        <v>0</v>
+      </c>
+      <c r="I458" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J458" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="n">
+        <v>2272</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E459" t="n">
+        <v>2</v>
+      </c>
+      <c r="F459" t="n">
+        <v>37903</v>
+      </c>
+      <c r="G459" t="n">
+        <v>111</v>
+      </c>
+      <c r="H459" t="n">
+        <v>0</v>
+      </c>
+      <c r="I459" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J459" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1" t="n">
+        <v>2273</v>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E460" t="n">
+        <v>3</v>
+      </c>
+      <c r="F460" t="n">
+        <v>37904</v>
+      </c>
+      <c r="G460" t="n">
+        <v>111</v>
+      </c>
+      <c r="H460" t="n">
+        <v>0</v>
+      </c>
+      <c r="I460" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J460" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1" t="n">
+        <v>2274</v>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E461" t="n">
+        <v>4</v>
+      </c>
+      <c r="F461" t="n">
+        <v>37905</v>
+      </c>
+      <c r="G461" t="n">
+        <v>222</v>
+      </c>
+      <c r="H461" t="n">
+        <v>0</v>
+      </c>
+      <c r="I461" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J461" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1" t="n">
+        <v>2275</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E462" t="n">
+        <v>1</v>
+      </c>
+      <c r="F462" t="n">
+        <v>37906</v>
+      </c>
+      <c r="G462" t="n">
+        <v>222</v>
+      </c>
+      <c r="H462" t="n">
+        <v>0</v>
+      </c>
+      <c r="I462" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J462" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1" t="n">
+        <v>2276</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E463" t="n">
+        <v>2</v>
+      </c>
+      <c r="F463" t="n">
+        <v>37907</v>
+      </c>
+      <c r="G463" t="n">
+        <v>111</v>
+      </c>
+      <c r="H463" t="n">
+        <v>0</v>
+      </c>
+      <c r="I463" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J463" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1" t="n">
+        <v>2277</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E464" t="n">
+        <v>3</v>
+      </c>
+      <c r="F464" t="n">
+        <v>37908</v>
+      </c>
+      <c r="G464" t="n">
+        <v>222</v>
+      </c>
+      <c r="H464" t="n">
+        <v>0</v>
+      </c>
+      <c r="I464" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J464" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1" t="n">
+        <v>2278</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E465" t="n">
+        <v>4</v>
+      </c>
+      <c r="F465" t="n">
+        <v>37909</v>
+      </c>
+      <c r="G465" t="n">
+        <v>222</v>
+      </c>
+      <c r="H465" t="n">
+        <v>0</v>
+      </c>
+      <c r="I465" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J465" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="1" t="n">
+        <v>2279</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E466" t="n">
+        <v>5</v>
+      </c>
+      <c r="F466" t="n">
+        <v>37910</v>
+      </c>
+      <c r="G466" t="n">
+        <v>25777</v>
+      </c>
+      <c r="H466" t="n">
+        <v>0.6186684640252704</v>
+      </c>
+      <c r="I466" t="n">
+        <v>105.1632360350992</v>
+      </c>
+      <c r="J466" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1" t="n">
+        <v>2280</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>FreeNav</t>
+        </is>
+      </c>
+      <c r="E467" t="n">
+        <v>1</v>
+      </c>
+      <c r="F467" t="n">
+        <v>38000</v>
+      </c>
+      <c r="G467" t="n">
+        <v>556</v>
+      </c>
+      <c r="H467" t="n">
+        <v>0</v>
+      </c>
+      <c r="I467" t="n">
+        <v>1.339285714285714</v>
+      </c>
+      <c r="J467" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1" t="n">
+        <v>2281</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="E468" t="n">
+        <v>1</v>
+      </c>
+      <c r="F468" t="n">
+        <v>38001</v>
+      </c>
+      <c r="G468" t="n">
+        <v>111</v>
+      </c>
+      <c r="H468" t="n">
+        <v>0</v>
+      </c>
+      <c r="I468" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="J468" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1" t="n">
+        <v>2282</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E469" t="n">
+        <v>1</v>
+      </c>
+      <c r="F469" t="n">
+        <v>38002</v>
+      </c>
+      <c r="G469" t="n">
+        <v>222</v>
+      </c>
+      <c r="H469" t="n">
+        <v>0</v>
+      </c>
+      <c r="I469" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J469" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1" t="n">
+        <v>2283</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E470" t="n">
+        <v>2</v>
+      </c>
+      <c r="F470" t="n">
+        <v>38003</v>
+      </c>
+      <c r="G470" t="n">
+        <v>111</v>
+      </c>
+      <c r="H470" t="n">
+        <v>0</v>
+      </c>
+      <c r="I470" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J470" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1" t="n">
+        <v>2284</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E471" t="n">
+        <v>3</v>
+      </c>
+      <c r="F471" t="n">
+        <v>38004</v>
+      </c>
+      <c r="G471" t="n">
+        <v>222</v>
+      </c>
+      <c r="H471" t="n">
+        <v>0</v>
+      </c>
+      <c r="I471" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J471" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="n">
+        <v>2285</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>VisibleTarget_1</t>
+        </is>
+      </c>
+      <c r="E472" t="n">
+        <v>4</v>
+      </c>
+      <c r="F472" t="n">
+        <v>38005</v>
+      </c>
+      <c r="G472" t="n">
+        <v>222</v>
+      </c>
+      <c r="H472" t="n">
+        <v>0</v>
+      </c>
+      <c r="I472" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J472" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="n">
+        <v>2286</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E473" t="n">
+        <v>1</v>
+      </c>
+      <c r="F473" t="n">
+        <v>38006</v>
+      </c>
+      <c r="G473" t="n">
+        <v>222</v>
+      </c>
+      <c r="H473" t="n">
+        <v>0</v>
+      </c>
+      <c r="I473" t="n">
+        <v>0.9616365727025896</v>
+      </c>
+      <c r="J473" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="n">
+        <v>2287</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E474" t="n">
+        <v>2</v>
+      </c>
+      <c r="F474" t="n">
+        <v>38007</v>
+      </c>
+      <c r="G474" t="n">
+        <v>111</v>
+      </c>
+      <c r="H474" t="n">
+        <v>0</v>
+      </c>
+      <c r="I474" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J474" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>2288</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E475" t="n">
+        <v>3</v>
+      </c>
+      <c r="F475" t="n">
+        <v>38008</v>
+      </c>
+      <c r="G475" t="n">
+        <v>111</v>
+      </c>
+      <c r="H475" t="n">
+        <v>0</v>
+      </c>
+      <c r="I475" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J475" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>2289</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E476" t="n">
+        <v>4</v>
+      </c>
+      <c r="F476" t="n">
+        <v>38009</v>
+      </c>
+      <c r="G476" t="n">
+        <v>111</v>
+      </c>
+      <c r="H476" t="n">
+        <v>0</v>
+      </c>
+      <c r="I476" t="n">
+        <v>0.4808182863512948</v>
+      </c>
+      <c r="J476" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>2290</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>Realidad Virtual</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>HiddenTarget_1</t>
+        </is>
+      </c>
+      <c r="E477" t="n">
+        <v>5</v>
+      </c>
+      <c r="F477" t="n">
+        <v>38010</v>
+      </c>
+      <c r="G477" t="n">
+        <v>556</v>
+      </c>
+      <c r="H477" t="n">
+        <v>0</v>
+      </c>
+      <c r="I477" t="n">
+        <v>2.404091431756474</v>
+      </c>
+      <c r="J477" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>